<commit_message>
Aggiornamento 2023 dopo nuovo check dati
</commit_message>
<xml_diff>
--- a/input/2023/wn.xlsx
+++ b/input/2023/wn.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.tora\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f.iapaolo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19845" windowHeight="14085" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2939" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2931" uniqueCount="407">
   <si>
     <t>AnnoBollettino</t>
   </si>
@@ -16242,10 +16242,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I326"/>
+  <dimension ref="A1:I324"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A240" sqref="A240:XFD240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23180,13 +23180,13 @@
         <v>87037</v>
       </c>
       <c r="F239" s="8">
-        <v>45050</v>
+        <v>0</v>
       </c>
       <c r="G239" s="3" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="H239" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I239" s="3">
         <v>1</v>
@@ -23200,13 +23200,13 @@
         <v>323</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E240" s="3">
-        <v>87037</v>
+        <v>81021</v>
       </c>
       <c r="F240" s="8">
         <v>0</v>
@@ -23226,25 +23226,25 @@
         <v>2023</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="C241" s="3" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="D241" s="3" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="E241" s="3">
-        <v>81021</v>
+        <v>28003</v>
       </c>
       <c r="F241" s="8">
-        <v>45190</v>
+        <v>45181</v>
       </c>
       <c r="G241" s="3" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="H241" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I241" s="3">
         <v>1</v>
@@ -23255,22 +23255,22 @@
         <v>2023</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="C242" s="3" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="D242" s="3" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="E242" s="3">
-        <v>81021</v>
+        <v>28011</v>
       </c>
       <c r="F242" s="8">
-        <v>0</v>
+        <v>45174</v>
       </c>
       <c r="G242" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H242" s="3">
         <v>1</v>
@@ -23290,16 +23290,16 @@
         <v>329</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E243" s="3">
-        <v>28003</v>
+        <v>28012</v>
       </c>
       <c r="F243" s="8">
-        <v>45181</v>
+        <v>45175</v>
       </c>
       <c r="G243" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H243" s="3">
         <v>1</v>
@@ -23319,13 +23319,13 @@
         <v>329</v>
       </c>
       <c r="D244" s="3" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E244" s="3">
-        <v>28011</v>
+        <v>28107</v>
       </c>
       <c r="F244" s="8">
-        <v>45174</v>
+        <v>45156</v>
       </c>
       <c r="G244" s="3" t="s">
         <v>404</v>
@@ -23348,13 +23348,13 @@
         <v>329</v>
       </c>
       <c r="D245" s="3" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E245" s="3">
-        <v>28012</v>
+        <v>28016</v>
       </c>
       <c r="F245" s="8">
-        <v>45175</v>
+        <v>45240</v>
       </c>
       <c r="G245" s="3" t="s">
         <v>406</v>
@@ -23377,13 +23377,13 @@
         <v>329</v>
       </c>
       <c r="D246" s="3" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="E246" s="3">
-        <v>28107</v>
+        <v>28017</v>
       </c>
       <c r="F246" s="8">
-        <v>45156</v>
+        <v>45169</v>
       </c>
       <c r="G246" s="3" t="s">
         <v>404</v>
@@ -23406,16 +23406,16 @@
         <v>329</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="E247" s="3">
-        <v>28016</v>
+        <v>28030</v>
       </c>
       <c r="F247" s="8">
-        <v>45240</v>
+        <v>45135</v>
       </c>
       <c r="G247" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H247" s="3">
         <v>1</v>
@@ -23435,16 +23435,16 @@
         <v>329</v>
       </c>
       <c r="D248" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E248" s="3">
-        <v>28017</v>
+        <v>28030</v>
       </c>
       <c r="F248" s="8">
-        <v>45169</v>
+        <v>45175</v>
       </c>
       <c r="G248" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H248" s="3">
         <v>1</v>
@@ -23470,10 +23470,10 @@
         <v>28030</v>
       </c>
       <c r="F249" s="8">
-        <v>45135</v>
+        <v>45188</v>
       </c>
       <c r="G249" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H249" s="3">
         <v>1</v>
@@ -23493,16 +23493,16 @@
         <v>329</v>
       </c>
       <c r="D250" s="3" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E250" s="3">
-        <v>28030</v>
+        <v>28037</v>
       </c>
       <c r="F250" s="8">
-        <v>45175</v>
+        <v>45155</v>
       </c>
       <c r="G250" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H250" s="3">
         <v>1</v>
@@ -23522,16 +23522,16 @@
         <v>329</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="E251" s="3">
-        <v>28030</v>
+        <v>28048</v>
       </c>
       <c r="F251" s="8">
-        <v>45188</v>
+        <v>45201</v>
       </c>
       <c r="G251" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H251" s="3">
         <v>1</v>
@@ -23551,13 +23551,13 @@
         <v>329</v>
       </c>
       <c r="D252" s="3" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E252" s="3">
-        <v>28037</v>
+        <v>28058</v>
       </c>
       <c r="F252" s="8">
-        <v>45155</v>
+        <v>45146</v>
       </c>
       <c r="G252" s="3" t="s">
         <v>404</v>
@@ -23580,13 +23580,13 @@
         <v>329</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="E253" s="3">
-        <v>28048</v>
+        <v>28060</v>
       </c>
       <c r="F253" s="8">
-        <v>45201</v>
+        <v>45138</v>
       </c>
       <c r="G253" s="3" t="s">
         <v>404</v>
@@ -23609,22 +23609,22 @@
         <v>329</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E254" s="3">
-        <v>28058</v>
+        <v>28060</v>
       </c>
       <c r="F254" s="8">
-        <v>45146</v>
+        <v>45143</v>
       </c>
       <c r="G254" s="3" t="s">
         <v>404</v>
       </c>
       <c r="H254" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I254" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.25">
@@ -23644,7 +23644,7 @@
         <v>28060</v>
       </c>
       <c r="F255" s="8">
-        <v>45138</v>
+        <v>45149</v>
       </c>
       <c r="G255" s="3" t="s">
         <v>404</v>
@@ -23673,16 +23673,16 @@
         <v>28060</v>
       </c>
       <c r="F256" s="8">
-        <v>45143</v>
+        <v>45150</v>
       </c>
       <c r="G256" s="3" t="s">
         <v>404</v>
       </c>
       <c r="H256" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I256" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.25">
@@ -23702,7 +23702,7 @@
         <v>28060</v>
       </c>
       <c r="F257" s="8">
-        <v>45149</v>
+        <v>45164</v>
       </c>
       <c r="G257" s="3" t="s">
         <v>404</v>
@@ -23731,10 +23731,10 @@
         <v>28060</v>
       </c>
       <c r="F258" s="8">
-        <v>45150</v>
+        <v>0</v>
       </c>
       <c r="G258" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H258" s="3">
         <v>1</v>
@@ -23754,19 +23754,19 @@
         <v>329</v>
       </c>
       <c r="D259" s="3" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="E259" s="3">
-        <v>28060</v>
+        <v>28086</v>
       </c>
       <c r="F259" s="8">
-        <v>45164</v>
+        <v>45127</v>
       </c>
       <c r="G259" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H259" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I259" s="3">
         <v>1</v>
@@ -23783,13 +23783,13 @@
         <v>329</v>
       </c>
       <c r="D260" s="3" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="E260" s="3">
-        <v>28060</v>
+        <v>28086</v>
       </c>
       <c r="F260" s="8">
-        <v>0</v>
+        <v>45129</v>
       </c>
       <c r="G260" s="3" t="s">
         <v>406</v>
@@ -23818,13 +23818,13 @@
         <v>28086</v>
       </c>
       <c r="F261" s="8">
-        <v>45127</v>
+        <v>45179</v>
       </c>
       <c r="G261" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H261" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I261" s="3">
         <v>1</v>
@@ -23841,16 +23841,16 @@
         <v>329</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E262" s="3">
-        <v>28086</v>
+        <v>28094</v>
       </c>
       <c r="F262" s="8">
-        <v>45129</v>
+        <v>45154</v>
       </c>
       <c r="G262" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H262" s="3">
         <v>1</v>
@@ -23870,16 +23870,16 @@
         <v>329</v>
       </c>
       <c r="D263" s="3" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="E263" s="3">
-        <v>28086</v>
+        <v>28105</v>
       </c>
       <c r="F263" s="8">
-        <v>45179</v>
+        <v>45170</v>
       </c>
       <c r="G263" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H263" s="3">
         <v>1</v>
@@ -23896,16 +23896,16 @@
         <v>328</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>329</v>
+        <v>350</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="E264" s="3">
-        <v>28094</v>
+        <v>29001</v>
       </c>
       <c r="F264" s="8">
-        <v>45154</v>
+        <v>45125</v>
       </c>
       <c r="G264" s="3" t="s">
         <v>405</v>
@@ -23925,19 +23925,19 @@
         <v>328</v>
       </c>
       <c r="C265" s="3" t="s">
-        <v>329</v>
+        <v>350</v>
       </c>
       <c r="D265" s="3" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E265" s="3">
-        <v>28105</v>
+        <v>29014</v>
       </c>
       <c r="F265" s="8">
-        <v>45170</v>
+        <v>45146</v>
       </c>
       <c r="G265" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H265" s="3">
         <v>1</v>
@@ -23957,13 +23957,13 @@
         <v>350</v>
       </c>
       <c r="D266" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E266" s="3">
-        <v>29001</v>
+        <v>29014</v>
       </c>
       <c r="F266" s="8">
-        <v>45125</v>
+        <v>45162</v>
       </c>
       <c r="G266" s="3" t="s">
         <v>405</v>
@@ -23986,13 +23986,13 @@
         <v>350</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E267" s="3">
-        <v>29014</v>
+        <v>29021</v>
       </c>
       <c r="F267" s="8">
-        <v>45146</v>
+        <v>45134</v>
       </c>
       <c r="G267" s="3" t="s">
         <v>405</v>
@@ -24015,13 +24015,13 @@
         <v>350</v>
       </c>
       <c r="D268" s="3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E268" s="3">
-        <v>29014</v>
+        <v>29039</v>
       </c>
       <c r="F268" s="8">
-        <v>45162</v>
+        <v>45154</v>
       </c>
       <c r="G268" s="3" t="s">
         <v>405</v>
@@ -24041,19 +24041,19 @@
         <v>328</v>
       </c>
       <c r="C269" s="3" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="D269" s="3" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="E269" s="3">
-        <v>29021</v>
+        <v>26008</v>
       </c>
       <c r="F269" s="8">
-        <v>45134</v>
+        <v>45168</v>
       </c>
       <c r="G269" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H269" s="3">
         <v>1</v>
@@ -24070,16 +24070,16 @@
         <v>328</v>
       </c>
       <c r="C270" s="3" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="D270" s="3" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="E270" s="3">
-        <v>29039</v>
+        <v>26058</v>
       </c>
       <c r="F270" s="8">
-        <v>45154</v>
+        <v>45134</v>
       </c>
       <c r="G270" s="3" t="s">
         <v>405</v>
@@ -24102,13 +24102,13 @@
         <v>355</v>
       </c>
       <c r="D271" s="3" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="E271" s="3">
-        <v>26008</v>
+        <v>26077</v>
       </c>
       <c r="F271" s="8">
-        <v>45168</v>
+        <v>45130</v>
       </c>
       <c r="G271" s="3" t="s">
         <v>406</v>
@@ -24128,16 +24128,16 @@
         <v>328</v>
       </c>
       <c r="C272" s="3" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="D272" s="3" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="E272" s="3">
-        <v>26058</v>
+        <v>27002</v>
       </c>
       <c r="F272" s="8">
-        <v>45134</v>
+        <v>45141</v>
       </c>
       <c r="G272" s="3" t="s">
         <v>405</v>
@@ -24157,19 +24157,19 @@
         <v>328</v>
       </c>
       <c r="C273" s="3" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="D273" s="3" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="E273" s="3">
-        <v>26077</v>
+        <v>27006</v>
       </c>
       <c r="F273" s="8">
-        <v>45130</v>
+        <v>45139</v>
       </c>
       <c r="G273" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H273" s="3">
         <v>1</v>
@@ -24189,16 +24189,16 @@
         <v>360</v>
       </c>
       <c r="D274" s="3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E274" s="3">
-        <v>27002</v>
+        <v>27006</v>
       </c>
       <c r="F274" s="8">
-        <v>45141</v>
+        <v>45164</v>
       </c>
       <c r="G274" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H274" s="3">
         <v>1</v>
@@ -24224,10 +24224,10 @@
         <v>27006</v>
       </c>
       <c r="F275" s="8">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="G275" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H275" s="3">
         <v>1</v>
@@ -24247,13 +24247,13 @@
         <v>360</v>
       </c>
       <c r="D276" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E276" s="3">
-        <v>27006</v>
+        <v>27008</v>
       </c>
       <c r="F276" s="8">
-        <v>45164</v>
+        <v>45133</v>
       </c>
       <c r="G276" s="3" t="s">
         <v>404</v>
@@ -24276,16 +24276,16 @@
         <v>360</v>
       </c>
       <c r="D277" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E277" s="3">
-        <v>27006</v>
+        <v>27008</v>
       </c>
       <c r="F277" s="8">
-        <v>45170</v>
+        <v>45154</v>
       </c>
       <c r="G277" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H277" s="3">
         <v>1</v>
@@ -24311,7 +24311,7 @@
         <v>27008</v>
       </c>
       <c r="F278" s="8">
-        <v>45133</v>
+        <v>45203</v>
       </c>
       <c r="G278" s="3" t="s">
         <v>404</v>
@@ -24334,19 +24334,19 @@
         <v>360</v>
       </c>
       <c r="D279" s="3" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E279" s="3">
-        <v>27008</v>
+        <v>27011</v>
       </c>
       <c r="F279" s="8">
-        <v>45154</v>
+        <v>45132</v>
       </c>
       <c r="G279" s="3" t="s">
         <v>405</v>
       </c>
       <c r="H279" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I279" s="3">
         <v>1</v>
@@ -24363,13 +24363,13 @@
         <v>360</v>
       </c>
       <c r="D280" s="3" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E280" s="3">
-        <v>27008</v>
+        <v>27011</v>
       </c>
       <c r="F280" s="8">
-        <v>45203</v>
+        <v>45139</v>
       </c>
       <c r="G280" s="3" t="s">
         <v>404</v>
@@ -24398,13 +24398,13 @@
         <v>27011</v>
       </c>
       <c r="F281" s="8">
-        <v>45132</v>
+        <v>45146</v>
       </c>
       <c r="G281" s="3" t="s">
         <v>405</v>
       </c>
       <c r="H281" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I281" s="3">
         <v>1</v>
@@ -24421,13 +24421,13 @@
         <v>360</v>
       </c>
       <c r="D282" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E282" s="3">
-        <v>27011</v>
+        <v>27013</v>
       </c>
       <c r="F282" s="8">
-        <v>45139</v>
+        <v>45133</v>
       </c>
       <c r="G282" s="3" t="s">
         <v>404</v>
@@ -24450,16 +24450,16 @@
         <v>360</v>
       </c>
       <c r="D283" s="3" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="E283" s="3">
-        <v>27011</v>
+        <v>27016</v>
       </c>
       <c r="F283" s="8">
-        <v>45146</v>
+        <v>45160</v>
       </c>
       <c r="G283" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H283" s="3">
         <v>1</v>
@@ -24479,13 +24479,13 @@
         <v>360</v>
       </c>
       <c r="D284" s="3" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E284" s="3">
-        <v>27013</v>
+        <v>27019</v>
       </c>
       <c r="F284" s="8">
-        <v>45133</v>
+        <v>45131</v>
       </c>
       <c r="G284" s="3" t="s">
         <v>404</v>
@@ -24508,13 +24508,13 @@
         <v>360</v>
       </c>
       <c r="D285" s="3" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="E285" s="3">
-        <v>27016</v>
+        <v>27020</v>
       </c>
       <c r="F285" s="8">
-        <v>45160</v>
+        <v>45169</v>
       </c>
       <c r="G285" s="3" t="s">
         <v>404</v>
@@ -24537,16 +24537,16 @@
         <v>360</v>
       </c>
       <c r="D286" s="3" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="E286" s="3">
-        <v>27019</v>
+        <v>27022</v>
       </c>
       <c r="F286" s="8">
-        <v>45131</v>
+        <v>45175</v>
       </c>
       <c r="G286" s="3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H286" s="3">
         <v>1</v>
@@ -24566,13 +24566,13 @@
         <v>360</v>
       </c>
       <c r="D287" s="3" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E287" s="3">
-        <v>27020</v>
+        <v>27023</v>
       </c>
       <c r="F287" s="8">
-        <v>45169</v>
+        <v>45170</v>
       </c>
       <c r="G287" s="3" t="s">
         <v>404</v>
@@ -24595,22 +24595,22 @@
         <v>360</v>
       </c>
       <c r="D288" s="3" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E288" s="3">
-        <v>27022</v>
+        <v>27023</v>
       </c>
       <c r="F288" s="8">
-        <v>45175</v>
+        <v>45196</v>
       </c>
       <c r="G288" s="3" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="H288" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I288" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.25">
@@ -24624,13 +24624,13 @@
         <v>360</v>
       </c>
       <c r="D289" s="3" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E289" s="3">
-        <v>27023</v>
+        <v>27024</v>
       </c>
       <c r="F289" s="8">
-        <v>45170</v>
+        <v>45147</v>
       </c>
       <c r="G289" s="3" t="s">
         <v>404</v>
@@ -24653,22 +24653,22 @@
         <v>360</v>
       </c>
       <c r="D290" s="3" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E290" s="3">
-        <v>27023</v>
+        <v>27024</v>
       </c>
       <c r="F290" s="8">
-        <v>45196</v>
+        <v>45159</v>
       </c>
       <c r="G290" s="3" t="s">
         <v>404</v>
       </c>
       <c r="H290" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I290" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.25">
@@ -24682,13 +24682,13 @@
         <v>360</v>
       </c>
       <c r="D291" s="3" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="E291" s="3">
-        <v>27024</v>
+        <v>27026</v>
       </c>
       <c r="F291" s="8">
-        <v>45147</v>
+        <v>45135</v>
       </c>
       <c r="G291" s="3" t="s">
         <v>404</v>
@@ -24711,16 +24711,16 @@
         <v>360</v>
       </c>
       <c r="D292" s="3" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="E292" s="3">
-        <v>27024</v>
+        <v>27031</v>
       </c>
       <c r="F292" s="8">
-        <v>45159</v>
+        <v>45174</v>
       </c>
       <c r="G292" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H292" s="3">
         <v>1</v>
@@ -24740,16 +24740,16 @@
         <v>360</v>
       </c>
       <c r="D293" s="3" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="E293" s="3">
-        <v>27026</v>
+        <v>27034</v>
       </c>
       <c r="F293" s="8">
-        <v>45135</v>
+        <v>45160</v>
       </c>
       <c r="G293" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H293" s="3">
         <v>1</v>
@@ -24769,16 +24769,16 @@
         <v>360</v>
       </c>
       <c r="D294" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E294" s="3">
-        <v>27031</v>
+        <v>27034</v>
       </c>
       <c r="F294" s="8">
-        <v>45174</v>
+        <v>45179</v>
       </c>
       <c r="G294" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H294" s="3">
         <v>1</v>
@@ -24798,16 +24798,16 @@
         <v>360</v>
       </c>
       <c r="D295" s="3" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E295" s="3">
-        <v>27034</v>
+        <v>27035</v>
       </c>
       <c r="F295" s="8">
-        <v>45160</v>
+        <v>45141</v>
       </c>
       <c r="G295" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H295" s="3">
         <v>1</v>
@@ -24827,16 +24827,16 @@
         <v>360</v>
       </c>
       <c r="D296" s="3" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="E296" s="3">
-        <v>27034</v>
+        <v>27039</v>
       </c>
       <c r="F296" s="8">
-        <v>45179</v>
+        <v>45110</v>
       </c>
       <c r="G296" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H296" s="3">
         <v>1</v>
@@ -24856,13 +24856,13 @@
         <v>360</v>
       </c>
       <c r="D297" s="3" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="E297" s="3">
-        <v>27035</v>
+        <v>27042</v>
       </c>
       <c r="F297" s="8">
-        <v>45141</v>
+        <v>45135</v>
       </c>
       <c r="G297" s="3" t="s">
         <v>404</v>
@@ -24885,16 +24885,16 @@
         <v>360</v>
       </c>
       <c r="D298" s="3" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="E298" s="3">
-        <v>27039</v>
+        <v>27042</v>
       </c>
       <c r="F298" s="8">
-        <v>45110</v>
+        <v>0</v>
       </c>
       <c r="G298" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H298" s="3">
         <v>1</v>
@@ -24920,10 +24920,10 @@
         <v>27042</v>
       </c>
       <c r="F299" s="8">
-        <v>45135</v>
+        <v>45142</v>
       </c>
       <c r="G299" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H299" s="3">
         <v>1</v>
@@ -24949,10 +24949,10 @@
         <v>27042</v>
       </c>
       <c r="F300" s="8">
-        <v>0</v>
+        <v>45174</v>
       </c>
       <c r="G300" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H300" s="3">
         <v>1</v>
@@ -24978,10 +24978,10 @@
         <v>27042</v>
       </c>
       <c r="F301" s="8">
-        <v>45142</v>
+        <v>45179</v>
       </c>
       <c r="G301" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H301" s="3">
         <v>1</v>
@@ -24998,19 +24998,19 @@
         <v>328</v>
       </c>
       <c r="C302" s="3" t="s">
-        <v>360</v>
+        <v>381</v>
       </c>
       <c r="D302" s="3" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="E302" s="3">
-        <v>27042</v>
+        <v>24056</v>
       </c>
       <c r="F302" s="8">
-        <v>45174</v>
+        <v>45189</v>
       </c>
       <c r="G302" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H302" s="3">
         <v>1</v>
@@ -25027,16 +25027,16 @@
         <v>328</v>
       </c>
       <c r="C303" s="3" t="s">
-        <v>360</v>
+        <v>383</v>
       </c>
       <c r="D303" s="3" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="E303" s="3">
-        <v>27042</v>
+        <v>23006</v>
       </c>
       <c r="F303" s="8">
-        <v>45179</v>
+        <v>45191</v>
       </c>
       <c r="G303" s="3" t="s">
         <v>404</v>
@@ -25056,19 +25056,19 @@
         <v>328</v>
       </c>
       <c r="C304" s="3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="D304" s="3" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="E304" s="3">
-        <v>24056</v>
+        <v>23019</v>
       </c>
       <c r="F304" s="8">
-        <v>45189</v>
+        <v>45139</v>
       </c>
       <c r="G304" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H304" s="3">
         <v>1</v>
@@ -25088,13 +25088,13 @@
         <v>383</v>
       </c>
       <c r="D305" s="3" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="E305" s="3">
-        <v>23006</v>
+        <v>23040</v>
       </c>
       <c r="F305" s="8">
-        <v>45191</v>
+        <v>45179</v>
       </c>
       <c r="G305" s="3" t="s">
         <v>404</v>
@@ -25117,16 +25117,16 @@
         <v>383</v>
       </c>
       <c r="D306" s="3" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E306" s="3">
-        <v>23019</v>
+        <v>23043</v>
       </c>
       <c r="F306" s="8">
-        <v>45139</v>
+        <v>45136</v>
       </c>
       <c r="G306" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H306" s="3">
         <v>1</v>
@@ -25146,16 +25146,16 @@
         <v>383</v>
       </c>
       <c r="D307" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E307" s="3">
-        <v>23040</v>
+        <v>23043</v>
       </c>
       <c r="F307" s="8">
-        <v>45179</v>
+        <v>45152</v>
       </c>
       <c r="G307" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H307" s="3">
         <v>1</v>
@@ -25181,7 +25181,7 @@
         <v>23043</v>
       </c>
       <c r="F308" s="8">
-        <v>45136</v>
+        <v>45224</v>
       </c>
       <c r="G308" s="3" t="s">
         <v>404</v>
@@ -25204,13 +25204,13 @@
         <v>383</v>
       </c>
       <c r="D309" s="3" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E309" s="3">
-        <v>23043</v>
+        <v>23044</v>
       </c>
       <c r="F309" s="8">
-        <v>45152</v>
+        <v>45144</v>
       </c>
       <c r="G309" s="3" t="s">
         <v>406</v>
@@ -25233,16 +25233,16 @@
         <v>383</v>
       </c>
       <c r="D310" s="3" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E310" s="3">
-        <v>23043</v>
+        <v>23044</v>
       </c>
       <c r="F310" s="8">
-        <v>45224</v>
+        <v>45151</v>
       </c>
       <c r="G310" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H310" s="3">
         <v>1</v>
@@ -25262,16 +25262,16 @@
         <v>383</v>
       </c>
       <c r="D311" s="3" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E311" s="3">
-        <v>23044</v>
+        <v>23050</v>
       </c>
       <c r="F311" s="8">
-        <v>45144</v>
+        <v>45179</v>
       </c>
       <c r="G311" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H311" s="3">
         <v>1</v>
@@ -25291,16 +25291,16 @@
         <v>383</v>
       </c>
       <c r="D312" s="3" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="E312" s="3">
-        <v>23044</v>
+        <v>23054</v>
       </c>
       <c r="F312" s="8">
-        <v>45151</v>
+        <v>45162</v>
       </c>
       <c r="G312" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H312" s="3">
         <v>1</v>
@@ -25320,13 +25320,13 @@
         <v>383</v>
       </c>
       <c r="D313" s="3" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="E313" s="3">
-        <v>23050</v>
+        <v>23055</v>
       </c>
       <c r="F313" s="8">
-        <v>45179</v>
+        <v>45152</v>
       </c>
       <c r="G313" s="3" t="s">
         <v>404</v>
@@ -25349,16 +25349,16 @@
         <v>383</v>
       </c>
       <c r="D314" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E314" s="3">
-        <v>23054</v>
+        <v>23055</v>
       </c>
       <c r="F314" s="8">
-        <v>45162</v>
+        <v>45200</v>
       </c>
       <c r="G314" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H314" s="3">
         <v>1</v>
@@ -25378,13 +25378,13 @@
         <v>383</v>
       </c>
       <c r="D315" s="3" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E315" s="3">
-        <v>23055</v>
+        <v>23059</v>
       </c>
       <c r="F315" s="8">
-        <v>45152</v>
+        <v>45179</v>
       </c>
       <c r="G315" s="3" t="s">
         <v>404</v>
@@ -25407,13 +25407,13 @@
         <v>383</v>
       </c>
       <c r="D316" s="3" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E316" s="3">
-        <v>23055</v>
+        <v>23059</v>
       </c>
       <c r="F316" s="8">
-        <v>45200</v>
+        <v>45224</v>
       </c>
       <c r="G316" s="3" t="s">
         <v>404</v>
@@ -25436,19 +25436,19 @@
         <v>383</v>
       </c>
       <c r="D317" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E317" s="3">
-        <v>23059</v>
+        <v>23064</v>
       </c>
       <c r="F317" s="8">
-        <v>45179</v>
+        <v>45120</v>
       </c>
       <c r="G317" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H317" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I317" s="3">
         <v>1</v>
@@ -25465,13 +25465,13 @@
         <v>383</v>
       </c>
       <c r="D318" s="3" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E318" s="3">
-        <v>23059</v>
+        <v>23071</v>
       </c>
       <c r="F318" s="8">
-        <v>45224</v>
+        <v>45152</v>
       </c>
       <c r="G318" s="3" t="s">
         <v>404</v>
@@ -25494,19 +25494,19 @@
         <v>383</v>
       </c>
       <c r="D319" s="3" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="E319" s="3">
-        <v>23064</v>
+        <v>23083</v>
       </c>
       <c r="F319" s="8">
-        <v>45120</v>
+        <v>45257</v>
       </c>
       <c r="G319" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H319" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I319" s="3">
         <v>1</v>
@@ -25523,10 +25523,10 @@
         <v>383</v>
       </c>
       <c r="D320" s="3" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="E320" s="3">
-        <v>23071</v>
+        <v>23091</v>
       </c>
       <c r="F320" s="8">
         <v>45152</v>
@@ -25552,13 +25552,13 @@
         <v>383</v>
       </c>
       <c r="D321" s="3" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="E321" s="3">
-        <v>23083</v>
+        <v>23091</v>
       </c>
       <c r="F321" s="8">
-        <v>45257</v>
+        <v>45179</v>
       </c>
       <c r="G321" s="3" t="s">
         <v>404</v>
@@ -25587,13 +25587,13 @@
         <v>23091</v>
       </c>
       <c r="F322" s="8">
-        <v>45152</v>
+        <v>45200</v>
       </c>
       <c r="G322" s="3" t="s">
         <v>404</v>
       </c>
       <c r="H322" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I322" s="3">
         <v>1</v>
@@ -25616,10 +25616,10 @@
         <v>23091</v>
       </c>
       <c r="F323" s="8">
-        <v>45179</v>
+        <v>45204</v>
       </c>
       <c r="G323" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H323" s="3">
         <v>1</v>
@@ -25639,79 +25639,21 @@
         <v>383</v>
       </c>
       <c r="D324" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E324" s="3">
-        <v>23091</v>
+        <v>23096</v>
       </c>
       <c r="F324" s="8">
-        <v>45200</v>
+        <v>45138</v>
       </c>
       <c r="G324" s="3" t="s">
         <v>404</v>
       </c>
       <c r="H324" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I324" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A325" s="3">
-        <v>2023</v>
-      </c>
-      <c r="B325" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="C325" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="D325" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="E325" s="3">
-        <v>23091</v>
-      </c>
-      <c r="F325" s="8">
-        <v>45204</v>
-      </c>
-      <c r="G325" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="H325" s="3">
-        <v>1</v>
-      </c>
-      <c r="I325" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A326" s="3">
-        <v>2023</v>
-      </c>
-      <c r="B326" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="C326" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="D326" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="E326" s="3">
-        <v>23096</v>
-      </c>
-      <c r="F326" s="8">
-        <v>45138</v>
-      </c>
-      <c r="G326" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="H326" s="3">
-        <v>1</v>
-      </c>
-      <c r="I326" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>